<commit_message>
used sun compass file for data entry
</commit_message>
<xml_diff>
--- a/sun_compass_correction.xlsx
+++ b/sun_compass_correction.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/0000_Github/SAM_Header/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d_user/0_GitHub/SAM_Header/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82403AD-F245-BA45-9FA7-BBDE394448B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596242C-FAB4-2640-B12F-CF5BC47B6277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25760" yWindow="5860" windowWidth="27640" windowHeight="16940" xr2:uid="{C43E5A99-261E-0848-8FDC-7C792A9583FD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8400" xr2:uid="{C43E5A99-261E-0848-8FDC-7C792A9583FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -40,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -385,23 +391,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776115F-8732-BF45-8D49-878DD5A268CB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -409,58 +415,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="B3">
         <f>IF(A3+90&gt;360,A3+90-360,A3+90)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
-        <v>318</v>
+        <v>232</v>
       </c>
       <c r="B4">
         <f>IF(A4+90&gt;360,A4+90-360,A4+90)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
-        <v>311</v>
+        <v>231</v>
       </c>
       <c r="B5">
         <f>IF(A5+90&gt;360,A5+90-360,A5+90)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6">
         <f>IF(A6+90&gt;360,A6+90-360,A6+90)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>275</v>
+      </c>
+      <c r="B7">
+        <f>IF(A7+90&gt;360,A7+90-360,A7+90)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="B8">
         <f>IF(A8+90&gt;360,A8+90-360,A8+90)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
-        <v>305</v>
+        <v>264</v>
       </c>
       <c r="B9">
         <f>IF(A9+90&gt;360,A9+90-360,A9+90)</f>
-        <v>35</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>268</v>
+      </c>
+      <c r="B10">
+        <f>IF(A10+90&gt;360,A10+90-360,A10+90)</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>264</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11" si="0">IF(A11+90&gt;360,A11+90-360,A11+90)</f>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>